<commit_message>
Added degree plans in SpreadSheet/Sample Data.xlsx
</commit_message>
<xml_diff>
--- a/SpreadSheet/Sample Data.xlsx
+++ b/SpreadSheet/Sample Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533569\Harshitha_Chetty_Ragava\44663\Mvc\SpreadSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sem 2\44663\Web application\Mvc\SpreadSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="103">
   <si>
     <t>CreditID</t>
   </si>
@@ -319,6 +319,21 @@
   </si>
   <si>
     <t>Summer 2018</t>
+  </si>
+  <si>
+    <t>Easy study plan</t>
+  </si>
+  <si>
+    <t>1 year plan</t>
+  </si>
+  <si>
+    <t>Study with break</t>
+  </si>
+  <si>
+    <t>Complete in one year</t>
+  </si>
+  <si>
+    <t>p</t>
   </si>
 </sst>
 </file>
@@ -1757,7 +1772,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -4554,15 +4571,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4615,6 +4632,40 @@
       </c>
       <c r="E3">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4">
+        <v>7253</v>
+      </c>
+      <c r="B4">
+        <v>533982</v>
+      </c>
+      <c r="C4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" customHeight="1">
+      <c r="A5">
+        <v>7254</v>
+      </c>
+      <c r="B5">
+        <v>533982</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -6677,7 +6728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -6891,34 +6944,618 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>7252</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <v>664</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>7252</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1">
+        <v>64</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>7252</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1">
+        <v>10</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" customHeight="1">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>7252</v>
+      </c>
+      <c r="C16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1">
+        <v>691</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" customHeight="1">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>7252</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>555</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" customHeight="1">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>7252</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2</v>
+      </c>
+      <c r="D18" s="1">
+        <v>618</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" customHeight="1">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>7252</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1">
+        <v>460</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" customHeight="1">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>7252</v>
+      </c>
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1">
+        <v>542</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>7252</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1">
+        <v>563</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>7252</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1">
+        <v>560</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>7252</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4</v>
+      </c>
+      <c r="D23" s="1">
+        <v>20</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>7252</v>
+      </c>
+      <c r="C24" s="1">
+        <v>4</v>
+      </c>
+      <c r="D24" s="1">
+        <v>692</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>7253</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>542</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>7253</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1</v>
+      </c>
+      <c r="D26" s="1">
+        <v>563</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>7253</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>460</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>7253</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>560</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>7253</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2</v>
+      </c>
+      <c r="D29" s="1">
+        <v>664</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>7253</v>
+      </c>
+      <c r="C30" s="1">
+        <v>2</v>
+      </c>
+      <c r="D30" s="1">
+        <v>64</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>7253</v>
+      </c>
+      <c r="C31" s="1">
+        <v>3</v>
+      </c>
+      <c r="D31" s="1">
+        <v>691</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>7253</v>
+      </c>
+      <c r="C32" s="1">
+        <v>3</v>
+      </c>
+      <c r="D32" s="1">
+        <v>10</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>7253</v>
+      </c>
+      <c r="C33" s="1">
+        <v>3</v>
+      </c>
+      <c r="D33" s="1">
+        <v>555</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>7253</v>
+      </c>
+      <c r="C34" s="1">
+        <v>4</v>
+      </c>
+      <c r="D34" s="1">
+        <v>692</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>7253</v>
+      </c>
+      <c r="C35" s="1">
+        <v>4</v>
+      </c>
+      <c r="D35" s="1">
+        <v>20</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>7253</v>
+      </c>
+      <c r="C36" s="1">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1">
+        <v>356</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>7254</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="1">
+        <v>460</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>7254</v>
+      </c>
+      <c r="C38" s="1">
+        <v>1</v>
+      </c>
+      <c r="D38" s="1">
+        <v>542</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>7254</v>
+      </c>
+      <c r="C39" s="1">
+        <v>1</v>
+      </c>
+      <c r="D39" s="1">
+        <v>356</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>7254</v>
+      </c>
+      <c r="C40" s="1">
+        <v>2</v>
+      </c>
+      <c r="D40" s="1">
+        <v>563</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>7254</v>
+      </c>
+      <c r="C41" s="1">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1">
+        <v>560</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>7254</v>
+      </c>
+      <c r="C42" s="1">
+        <v>2</v>
+      </c>
+      <c r="D42" s="1">
+        <v>664</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>7254</v>
+      </c>
+      <c r="C43" s="1">
+        <v>3</v>
+      </c>
+      <c r="D43" s="1">
+        <v>618</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>7254</v>
+      </c>
+      <c r="C44" s="1">
+        <v>3</v>
+      </c>
+      <c r="D44" s="1">
+        <v>555</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>7254</v>
+      </c>
+      <c r="C45" s="1">
+        <v>3</v>
+      </c>
+      <c r="D45" s="1">
+        <v>691</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>7254</v>
+      </c>
+      <c r="C46" s="1">
+        <v>4</v>
+      </c>
+      <c r="D46" s="1">
+        <v>692</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>7254</v>
+      </c>
+      <c r="C47" s="1">
+        <v>4</v>
+      </c>
+      <c r="D47" s="1">
+        <v>10</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>7254</v>
+      </c>
+      <c r="C48" s="1">
+        <v>4</v>
+      </c>
+      <c r="D48" s="1">
+        <v>64</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
     <row r="49" ht="15.75" customHeight="1"/>
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1"/>
@@ -7881,7 +8518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
nuka degree SpreadSheet commit
</commit_message>
<xml_diff>
--- a/SpreadSheet/Sample Data.xlsx
+++ b/SpreadSheet/Sample Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sem 2\44663\Web application\Mvc\SpreadSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533573\Documents\44663\New folder\Mvc\SpreadSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="107">
   <si>
     <t>CreditID</t>
   </si>
@@ -335,12 +335,24 @@
   <si>
     <t>p</t>
   </si>
+  <si>
+    <t>slow and steady</t>
+  </si>
+  <si>
+    <t>Default fall plan</t>
+  </si>
+  <si>
+    <t>Maximum semester possible</t>
+  </si>
+  <si>
+    <t>Fall intake default 1.5 year plan.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -360,6 +372,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -400,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -431,6 +449,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4571,15 +4590,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
     <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4666,6 +4685,40 @@
       </c>
       <c r="E5">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1">
+      <c r="A6">
+        <v>7255</v>
+      </c>
+      <c r="B6">
+        <v>533573</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" customHeight="1">
+      <c r="A7">
+        <v>7256</v>
+      </c>
+      <c r="B7">
+        <v>533573</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -6728,7 +6781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
@@ -8518,7 +8571,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -11906,6 +11961,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
I have seeded DegreeCredit and DegreePlan domain Models.
</commit_message>
<xml_diff>
--- a/SpreadSheet/Sample Data.xlsx
+++ b/SpreadSheet/Sample Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533569\Harshitha_Chetty_Ragava\44663\Mvc\SpreadSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sem 2\44663\Web application\Mvc\SpreadSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -222,9 +222,6 @@
     <t>Maximum semester possible</t>
   </si>
   <si>
-    <t>Fall intake default 1.5 year plan.</t>
-  </si>
-  <si>
     <t>Android</t>
   </si>
   <si>
@@ -328,6 +325,9 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>Default one and half year plan</t>
   </si>
 </sst>
 </file>
@@ -745,7 +745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -761,7 +761,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -770,10 +770,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1855,22 +1855,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1918,7 +1918,7 @@
         <v>542</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>14</v>
@@ -1938,7 +1938,7 @@
         <v>563</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>15</v>
@@ -2078,10 +2078,10 @@
         <v>643</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D12" s="12">
         <v>0</v>
@@ -2138,10 +2138,10 @@
         <v>644</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D15" s="12">
         <v>0</v>
@@ -3147,7 +3147,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -3162,13 +3162,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -4660,8 +4660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4676,19 +4676,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -4705,7 +4705,7 @@
         <v>34</v>
       </c>
       <c r="E2" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -4722,7 +4722,7 @@
         <v>37</v>
       </c>
       <c r="E3" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1">
@@ -4787,10 +4787,10 @@
         <v>63</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="E7" s="12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -5799,19 +5799,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -6871,19 +6871,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -9055,19 +9055,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -9305,7 +9305,7 @@
         <v>51</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:5">

</xml_diff>

<commit_message>
Seeded Student term domain model
</commit_message>
<xml_diff>
--- a/SpreadSheet/Sample Data.xlsx
+++ b/SpreadSheet/Sample Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sem 2\44663\Web application\Mvc\SpreadSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533573\Documents\44663\New folder\Mvc\SpreadSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -4660,7 +4660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -9040,8 +9040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9157,7 +9157,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B7" s="5">
         <v>533982</v>
@@ -9174,7 +9174,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B8" s="5">
         <v>533982</v>
@@ -9191,7 +9191,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="5">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5">
         <v>533982</v>
@@ -9208,7 +9208,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="5">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5">
         <v>533982</v>
@@ -9225,7 +9225,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B11" s="5">
         <v>533982</v>
@@ -9242,7 +9242,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B12" s="6">
         <v>533573</v>
@@ -9259,7 +9259,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B13" s="6">
         <v>533573</v>
@@ -9276,7 +9276,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B14" s="6">
         <v>533573</v>
@@ -9293,7 +9293,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="6">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B15" s="6">
         <v>533573</v>
@@ -9310,7 +9310,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="6">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B16" s="6">
         <v>533573</v>

</xml_diff>

<commit_message>
Successfully updated tables with FK's.
</commit_message>
<xml_diff>
--- a/SpreadSheet/Sample Data.xlsx
+++ b/SpreadSheet/Sample Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533573\Documents\44663\New folder\Mvc\SpreadSheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533569\Harshitha_Chetty_Ragava\44663\Mvc\SpreadSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20415" windowHeight="7590" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="103">
   <si>
     <t>DB</t>
   </si>
@@ -294,9 +294,6 @@
     <t>919(U,15)</t>
   </si>
   <si>
-    <t>SlotID(PK)(U,5)</t>
-  </si>
-  <si>
     <t>Term(U,2)</t>
   </si>
   <si>
@@ -321,13 +318,22 @@
     <t>Fall2019</t>
   </si>
   <si>
-    <t>DegreePlanID(FK)(U,5)</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
     <t>Default one and half year plan</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>SlotId(PK)(U,5)</t>
+  </si>
+  <si>
+    <t>DegreePlanId(FK)(U,5)</t>
+  </si>
+  <si>
+    <t>CreditId(FK)(U,5)</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -463,6 +469,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -773,7 +780,7 @@
         <v>70</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -790,8 +797,8 @@
         <v>5</v>
       </c>
       <c r="E2" t="str">
-        <f>" new Degree {" &amp;$A$1 &amp; "=" &amp; A2 &amp;","&amp;$B$1 &amp; "=" &amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp; "},"</f>
-        <v xml:space="preserve"> new Degree {DegreeID(PK)(U,5)=1,DegreeAbrrev(U,8)=ACS+2,DegreeName(U,20)=MS ACS + 2 },</v>
+        <f>" new Degree {" &amp;$A$1 &amp; "=" &amp; A2 &amp;","&amp;$B$1 &amp; "="&amp;"'"&amp;B2&amp;"'"&amp;","&amp;$C$1&amp;"="&amp;C2&amp; "},"</f>
+        <v xml:space="preserve"> new Degree {DegreeID(PK)(U,5)=1,DegreeAbrrev(U,8)='ACS+2',DegreeName(U,20)=MS ACS + 2 },</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -808,8 +815,8 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f t="shared" ref="E3:E5" si="0">" new Degree {" &amp;$A$1 &amp; "=" &amp; A3 &amp;","&amp;$B$1 &amp; "=" &amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp; "},"</f>
-        <v xml:space="preserve"> new Degree {DegreeID(PK)(U,5)=2,DegreeAbrrev(U,8)=ACS+DB,DegreeName(U,20)=MS ACS + DB},</v>
+        <f t="shared" ref="E3:E5" si="0">" new Degree {" &amp;$A$1 &amp; "=" &amp; A3 &amp;","&amp;$B$1 &amp; "="&amp;"'"&amp;B3&amp;"'"&amp;","&amp;$C$1&amp;"="&amp;C3&amp; "},"</f>
+        <v xml:space="preserve"> new Degree {DegreeID(PK)(U,5)=2,DegreeAbrrev(U,8)='ACS+DB',DegreeName(U,20)=MS ACS + DB},</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -827,7 +834,7 @@
       </c>
       <c r="E4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Degree {DegreeID(PK)(U,5)=3,DegreeAbrrev(U,8)=ACS+NF,DegreeName(U,20)=MS ACS + NF},</v>
+        <v xml:space="preserve"> new Degree {DegreeID(PK)(U,5)=3,DegreeAbrrev(U,8)='ACS+NF',DegreeName(U,20)=MS ACS + NF},</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -845,7 +852,7 @@
       </c>
       <c r="E5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> new Degree {DegreeID(PK)(U,5)=4,DegreeAbrrev(U,8)=ACS,DegreeName(U,20)=MS ACS},</v>
+        <v xml:space="preserve"> new Degree {DegreeID(PK)(U,5)=4,DegreeAbrrev(U,8)='ACS',DegreeName(U,20)=MS ACS},</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -4679,7 +4686,7 @@
         <v>81</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>82</v>
@@ -4787,7 +4794,7 @@
         <v>63</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E7" s="12">
         <v>3</v>
@@ -6853,10 +6860,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E999"/>
+  <dimension ref="A1:F999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -6866,27 +6873,31 @@
     <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="26" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="102.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -6902,8 +6913,12 @@
       <c r="E2" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="str">
+        <f xml:space="preserve"> " new Slot {"&amp;$A$1&amp;"="&amp;A2&amp;","&amp;$B$1&amp;"="&amp;B2&amp;","&amp;$C$1&amp;"="&amp;C2&amp;","&amp;$D$1&amp;"="&amp;D2&amp;","&amp;$E$1&amp;"="&amp;"'"&amp;E2&amp; "'"&amp;"},"</f>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=1,DegreePlanId(FK)(U,5)=7251,Term(U,2)=1,CreditId(FK)(U,5)=542,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -6919,8 +6934,12 @@
       <c r="E3" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="1" t="str">
+        <f xml:space="preserve"> " new Slot {"&amp;$A$1&amp;"="&amp;A3&amp;","&amp;$B$1&amp;"="&amp;B3&amp;","&amp;$C$1&amp;"="&amp;C3&amp;","&amp;$D$1&amp;"="&amp;D3&amp;","&amp;$E$1&amp;"="&amp;"'"&amp;E3&amp; "'"&amp;"},"</f>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=2,DegreePlanId(FK)(U,5)=7251,Term(U,2)=1,CreditId(FK)(U,5)=563,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -6936,8 +6955,12 @@
       <c r="E4" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="1" t="str">
+        <f t="shared" ref="F4:F67" si="0" xml:space="preserve"> " new Slot {"&amp;$A$1&amp;"="&amp;A4&amp;","&amp;$B$1&amp;"="&amp;B4&amp;","&amp;$C$1&amp;"="&amp;C4&amp;","&amp;$D$1&amp;"="&amp;D4&amp;","&amp;$E$1&amp;"="&amp;"'"&amp;E4&amp; "'"&amp;"},"</f>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=3,DegreePlanId(FK)(U,5)=7251,Term(U,2)=1,CreditId(FK)(U,5)=560,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -6953,8 +6976,12 @@
       <c r="E5" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=4,DegreePlanId(FK)(U,5)=7251,Term(U,2)=2,CreditId(FK)(U,5)=664,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -6970,8 +6997,12 @@
       <c r="E6" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=5,DegreePlanId(FK)(U,5)=7251,Term(U,2)=2,CreditId(FK)(U,5)=6,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -6987,8 +7018,12 @@
       <c r="E7" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=6,DegreePlanId(FK)(U,5)=7251,Term(U,2)=2,CreditId(FK)(U,5)=10,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -7004,8 +7039,12 @@
       <c r="E8" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=7,DegreePlanId(FK)(U,5)=7251,Term(U,2)=3,CreditId(FK)(U,5)=618,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -7021,8 +7060,12 @@
       <c r="E9" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=8,DegreePlanId(FK)(U,5)=7251,Term(U,2)=3,CreditId(FK)(U,5)=691,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -7038,8 +7081,12 @@
       <c r="E10" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=9,DegreePlanId(FK)(U,5)=7251,Term(U,2)=4,CreditId(FK)(U,5)=692,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -7055,8 +7102,12 @@
       <c r="E11" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=10,DegreePlanId(FK)(U,5)=7251,Term(U,2)=4,CreditId(FK)(U,5)=20,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="12">
         <v>11</v>
       </c>
@@ -7072,8 +7123,12 @@
       <c r="E12" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="F12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=11,DegreePlanId(FK)(U,5)=7251,Term(U,2)=4,CreditId(FK)(U,5)=555,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" customHeight="1">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -7089,8 +7144,12 @@
       <c r="E13" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1">
+      <c r="F13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=12,DegreePlanId(FK)(U,5)=7252,Term(U,2)=1,CreditId(FK)(U,5)=664,Status(U,1)='p'},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -7106,8 +7165,12 @@
       <c r="E14" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" customHeight="1">
+      <c r="F14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=13,DegreePlanId(FK)(U,5)=7252,Term(U,2)=1,CreditId(FK)(U,5)=64,Status(U,1)='p'},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" customHeight="1">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -7123,8 +7186,12 @@
       <c r="E15" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1">
+      <c r="F15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=14,DegreePlanId(FK)(U,5)=7252,Term(U,2)=1,CreditId(FK)(U,5)=10,Status(U,1)='p'},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" customHeight="1">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -7140,8 +7207,12 @@
       <c r="E16" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1">
+      <c r="F16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=15,DegreePlanId(FK)(U,5)=7252,Term(U,2)=2,CreditId(FK)(U,5)=691,Status(U,1)='p'},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -7157,8 +7228,12 @@
       <c r="E17" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1">
+      <c r="F17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=16,DegreePlanId(FK)(U,5)=7252,Term(U,2)=2,CreditId(FK)(U,5)=555,Status(U,1)='p'},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -7174,8 +7249,12 @@
       <c r="E18" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1">
+      <c r="F18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=17,DegreePlanId(FK)(U,5)=7252,Term(U,2)=2,CreditId(FK)(U,5)=618,Status(U,1)='p'},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -7191,8 +7270,12 @@
       <c r="E19" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1">
+      <c r="F19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=18,DegreePlanId(FK)(U,5)=7252,Term(U,2)=3,CreditId(FK)(U,5)=460,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -7208,8 +7291,12 @@
       <c r="E20" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=19,DegreePlanId(FK)(U,5)=7252,Term(U,2)=3,CreditId(FK)(U,5)=542,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="12">
         <v>20</v>
       </c>
@@ -7225,8 +7312,12 @@
       <c r="E21" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=20,DegreePlanId(FK)(U,5)=7252,Term(U,2)=3,CreditId(FK)(U,5)=563,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="12">
         <v>21</v>
       </c>
@@ -7242,8 +7333,12 @@
       <c r="E22" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=21,DegreePlanId(FK)(U,5)=7252,Term(U,2)=4,CreditId(FK)(U,5)=560,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="A23" s="12">
         <v>22</v>
       </c>
@@ -7259,8 +7354,12 @@
       <c r="E23" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=22,DegreePlanId(FK)(U,5)=7252,Term(U,2)=4,CreditId(FK)(U,5)=20,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="12">
         <v>23</v>
       </c>
@@ -7276,8 +7375,12 @@
       <c r="E24" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=23,DegreePlanId(FK)(U,5)=7252,Term(U,2)=4,CreditId(FK)(U,5)=692,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="12">
         <v>24</v>
       </c>
@@ -7293,8 +7396,12 @@
       <c r="E25" s="13" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=24,DegreePlanId(FK)(U,5)=7253,Term(U,2)=1,CreditId(FK)(U,5)=542,Status(U,1)='p'},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="12">
         <v>25</v>
       </c>
@@ -7310,8 +7417,12 @@
       <c r="E26" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=25,DegreePlanId(FK)(U,5)=7253,Term(U,2)=1,CreditId(FK)(U,5)=563,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27" s="12">
         <v>26</v>
       </c>
@@ -7327,8 +7438,12 @@
       <c r="E27" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=26,DegreePlanId(FK)(U,5)=7253,Term(U,2)=1,CreditId(FK)(U,5)=460,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28" s="12">
         <v>27</v>
       </c>
@@ -7344,8 +7459,12 @@
       <c r="E28" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=27,DegreePlanId(FK)(U,5)=7253,Term(U,2)=2,CreditId(FK)(U,5)=560,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29" s="12">
         <v>28</v>
       </c>
@@ -7361,8 +7480,12 @@
       <c r="E29" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=28,DegreePlanId(FK)(U,5)=7253,Term(U,2)=2,CreditId(FK)(U,5)=664,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30" s="12">
         <v>29</v>
       </c>
@@ -7378,8 +7501,12 @@
       <c r="E30" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=29,DegreePlanId(FK)(U,5)=7253,Term(U,2)=2,CreditId(FK)(U,5)=64,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="12">
         <v>30</v>
       </c>
@@ -7395,8 +7522,12 @@
       <c r="E31" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=30,DegreePlanId(FK)(U,5)=7253,Term(U,2)=3,CreditId(FK)(U,5)=691,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32" s="12">
         <v>31</v>
       </c>
@@ -7412,8 +7543,12 @@
       <c r="E32" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=31,DegreePlanId(FK)(U,5)=7253,Term(U,2)=3,CreditId(FK)(U,5)=10,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15.75" customHeight="1">
       <c r="A33" s="12">
         <v>32</v>
       </c>
@@ -7429,8 +7564,12 @@
       <c r="E33" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=32,DegreePlanId(FK)(U,5)=7253,Term(U,2)=3,CreditId(FK)(U,5)=555,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" customHeight="1">
       <c r="A34" s="12">
         <v>33</v>
       </c>
@@ -7446,8 +7585,12 @@
       <c r="E34" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=33,DegreePlanId(FK)(U,5)=7253,Term(U,2)=4,CreditId(FK)(U,5)=692,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" customHeight="1">
       <c r="A35" s="12">
         <v>34</v>
       </c>
@@ -7463,8 +7606,12 @@
       <c r="E35" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=34,DegreePlanId(FK)(U,5)=7253,Term(U,2)=4,CreditId(FK)(U,5)=20,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15.75" customHeight="1">
       <c r="A36" s="12">
         <v>35</v>
       </c>
@@ -7480,8 +7627,12 @@
       <c r="E36" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=35,DegreePlanId(FK)(U,5)=7253,Term(U,2)=4,CreditId(FK)(U,5)=356,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15.75" customHeight="1">
       <c r="A37" s="12">
         <v>36</v>
       </c>
@@ -7497,8 +7648,12 @@
       <c r="E37" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=36,DegreePlanId(FK)(U,5)=7254,Term(U,2)=1,CreditId(FK)(U,5)=460,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15.75" customHeight="1">
       <c r="A38" s="12">
         <v>37</v>
       </c>
@@ -7514,8 +7669,12 @@
       <c r="E38" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=37,DegreePlanId(FK)(U,5)=7254,Term(U,2)=1,CreditId(FK)(U,5)=542,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15.75" customHeight="1">
       <c r="A39" s="12">
         <v>38</v>
       </c>
@@ -7531,8 +7690,12 @@
       <c r="E39" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=38,DegreePlanId(FK)(U,5)=7254,Term(U,2)=1,CreditId(FK)(U,5)=356,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15.75" customHeight="1">
       <c r="A40" s="12">
         <v>39</v>
       </c>
@@ -7548,8 +7711,12 @@
       <c r="E40" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=39,DegreePlanId(FK)(U,5)=7254,Term(U,2)=2,CreditId(FK)(U,5)=563,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="15.75" customHeight="1">
       <c r="A41" s="12">
         <v>40</v>
       </c>
@@ -7565,8 +7732,12 @@
       <c r="E41" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=40,DegreePlanId(FK)(U,5)=7254,Term(U,2)=2,CreditId(FK)(U,5)=560,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1">
       <c r="A42" s="12">
         <v>41</v>
       </c>
@@ -7582,8 +7753,12 @@
       <c r="E42" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=41,DegreePlanId(FK)(U,5)=7254,Term(U,2)=2,CreditId(FK)(U,5)=664,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1">
       <c r="A43" s="12">
         <v>42</v>
       </c>
@@ -7599,8 +7774,12 @@
       <c r="E43" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=42,DegreePlanId(FK)(U,5)=7254,Term(U,2)=3,CreditId(FK)(U,5)=618,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1">
       <c r="A44" s="12">
         <v>43</v>
       </c>
@@ -7616,8 +7795,12 @@
       <c r="E44" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=43,DegreePlanId(FK)(U,5)=7254,Term(U,2)=3,CreditId(FK)(U,5)=555,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1">
       <c r="A45" s="12">
         <v>44</v>
       </c>
@@ -7633,8 +7816,12 @@
       <c r="E45" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=44,DegreePlanId(FK)(U,5)=7254,Term(U,2)=3,CreditId(FK)(U,5)=691,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="15.75" customHeight="1">
       <c r="A46" s="12">
         <v>45</v>
       </c>
@@ -7650,8 +7837,12 @@
       <c r="E46" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=45,DegreePlanId(FK)(U,5)=7254,Term(U,2)=4,CreditId(FK)(U,5)=692,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="15.75" customHeight="1">
       <c r="A47" s="12">
         <v>46</v>
       </c>
@@ -7667,8 +7858,12 @@
       <c r="E47" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=46,DegreePlanId(FK)(U,5)=7254,Term(U,2)=4,CreditId(FK)(U,5)=10,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="15.75" customHeight="1">
       <c r="A48" s="12">
         <v>47</v>
       </c>
@@ -7684,8 +7879,12 @@
       <c r="E48" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=47,DegreePlanId(FK)(U,5)=7254,Term(U,2)=4,CreditId(FK)(U,5)=64,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15.75" customHeight="1">
       <c r="A49" s="12">
         <v>48</v>
       </c>
@@ -7701,8 +7900,12 @@
       <c r="E49" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=48,DegreePlanId(FK)(U,5)=7255,Term(U,2)=1,CreditId(FK)(U,5)=356,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15.75" customHeight="1">
       <c r="A50" s="12">
         <v>49</v>
       </c>
@@ -7718,8 +7921,12 @@
       <c r="E50" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=49,DegreePlanId(FK)(U,5)=7255,Term(U,2)=1,CreditId(FK)(U,5)=563,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15.75" customHeight="1">
       <c r="A51" s="12">
         <v>50</v>
       </c>
@@ -7735,8 +7942,12 @@
       <c r="E51" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=50,DegreePlanId(FK)(U,5)=7255,Term(U,2)=1,CreditId(FK)(U,5)=542,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" customHeight="1">
       <c r="A52" s="12">
         <v>51</v>
       </c>
@@ -7752,8 +7963,12 @@
       <c r="E52" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=51,DegreePlanId(FK)(U,5)=7255,Term(U,2)=2,CreditId(FK)(U,5)=555,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15.75" customHeight="1">
       <c r="A53" s="12">
         <v>52</v>
       </c>
@@ -7769,8 +7984,12 @@
       <c r="E53" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=52,DegreePlanId(FK)(U,5)=7255,Term(U,2)=2,CreditId(FK)(U,5)=644,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15.75" customHeight="1">
       <c r="A54" s="12">
         <v>53</v>
       </c>
@@ -7786,8 +8005,12 @@
       <c r="E54" s="13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=53,DegreePlanId(FK)(U,5)=7255,Term(U,2)=2,CreditId(FK)(U,5)=560,Status(U,1)='C'},</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1">
       <c r="A55" s="12">
         <v>54</v>
       </c>
@@ -7803,8 +8026,12 @@
       <c r="E55" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=54,DegreePlanId(FK)(U,5)=7255,Term(U,2)=3,CreditId(FK)(U,5)=618,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="15.75" customHeight="1">
       <c r="A56" s="12">
         <v>55</v>
       </c>
@@ -7820,8 +8047,12 @@
       <c r="E56" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F56" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=55,DegreePlanId(FK)(U,5)=7255,Term(U,2)=3,CreditId(FK)(U,5)=691,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1">
       <c r="A57" s="12">
         <v>56</v>
       </c>
@@ -7837,8 +8068,12 @@
       <c r="E57" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F57" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=56,DegreePlanId(FK)(U,5)=7255,Term(U,2)=4,CreditId(FK)(U,5)=692,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" customHeight="1">
       <c r="A58" s="12">
         <v>57</v>
       </c>
@@ -7854,8 +8089,12 @@
       <c r="E58" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F58" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=57,DegreePlanId(FK)(U,5)=7255,Term(U,2)=4,CreditId(FK)(U,5)=643,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" customHeight="1">
       <c r="A59" s="12">
         <v>58</v>
       </c>
@@ -7871,8 +8110,12 @@
       <c r="E59" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" ht="15" customHeight="1">
+      <c r="F59" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=58,DegreePlanId(FK)(U,5)=7255,Term(U,2)=4,CreditId(FK)(U,5)=10,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15" customHeight="1">
       <c r="A60" s="12">
         <v>59</v>
       </c>
@@ -7888,8 +8131,12 @@
       <c r="E60" s="14" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F60" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=59,DegreePlanId(FK)(U,5)=7255,Term(U,2)=5,CreditId(FK)(U,5)=664,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="15.75" customHeight="1">
       <c r="A61" s="12">
         <v>60</v>
       </c>
@@ -7905,8 +8152,12 @@
       <c r="E61" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F61" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=60,DegreePlanId(FK)(U,5)=7256,Term(U,2)=1,CreditId(FK)(U,5)=356,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="15.75" customHeight="1">
       <c r="A62" s="12">
         <v>61</v>
       </c>
@@ -7922,8 +8173,12 @@
       <c r="E62" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F62" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=61,DegreePlanId(FK)(U,5)=7256,Term(U,2)=1,CreditId(FK)(U,5)=563,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="15.75" customHeight="1">
       <c r="A63" s="12">
         <v>62</v>
       </c>
@@ -7939,8 +8194,12 @@
       <c r="E63" s="13" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F63" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=62,DegreePlanId(FK)(U,5)=7256,Term(U,2)=1,CreditId(FK)(U,5)=542,Status(U,1)='A'},</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="15.75" customHeight="1">
       <c r="A64" s="12">
         <v>63</v>
       </c>
@@ -7956,8 +8215,12 @@
       <c r="E64" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F64" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=63,DegreePlanId(FK)(U,5)=7256,Term(U,2)=2,CreditId(FK)(U,5)=555,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="15.75" customHeight="1">
       <c r="A65" s="12">
         <v>64</v>
       </c>
@@ -7973,8 +8236,12 @@
       <c r="E65" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F65" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=64,DegreePlanId(FK)(U,5)=7256,Term(U,2)=2,CreditId(FK)(U,5)=644,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="15.75" customHeight="1">
       <c r="A66" s="12">
         <v>65</v>
       </c>
@@ -7990,8 +8257,12 @@
       <c r="E66" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F66" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=65,DegreePlanId(FK)(U,5)=7256,Term(U,2)=2,CreditId(FK)(U,5)=560,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15.75" customHeight="1">
       <c r="A67" s="12">
         <v>66</v>
       </c>
@@ -8007,8 +8278,12 @@
       <c r="E67" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F67" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=66,DegreePlanId(FK)(U,5)=7256,Term(U,2)=3,CreditId(FK)(U,5)=618,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="15.75" customHeight="1">
       <c r="A68" s="12">
         <v>67</v>
       </c>
@@ -8024,8 +8299,12 @@
       <c r="E68" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F68" s="1" t="str">
+        <f t="shared" ref="F68:F72" si="1" xml:space="preserve"> " new Slot {"&amp;$A$1&amp;"="&amp;A68&amp;","&amp;$B$1&amp;"="&amp;B68&amp;","&amp;$C$1&amp;"="&amp;C68&amp;","&amp;$D$1&amp;"="&amp;D68&amp;","&amp;$E$1&amp;"="&amp;"'"&amp;E68&amp; "'"&amp;"},"</f>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=67,DegreePlanId(FK)(U,5)=7256,Term(U,2)=3,CreditId(FK)(U,5)=691,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="15.75" customHeight="1">
       <c r="A69" s="12">
         <v>68</v>
       </c>
@@ -8041,8 +8320,12 @@
       <c r="E69" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F69" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=68,DegreePlanId(FK)(U,5)=7256,Term(U,2)=4,CreditId(FK)(U,5)=692,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15.75" customHeight="1">
       <c r="A70" s="12">
         <v>69</v>
       </c>
@@ -8058,8 +8341,12 @@
       <c r="E70" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F70" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=69,DegreePlanId(FK)(U,5)=7256,Term(U,2)=4,CreditId(FK)(U,5)=643,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" customHeight="1">
       <c r="A71" s="12">
         <v>70</v>
       </c>
@@ -8075,8 +8362,12 @@
       <c r="E71" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F71" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=70,DegreePlanId(FK)(U,5)=7256,Term(U,2)=5,CreditId(FK)(U,5)=10,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="15.75" customHeight="1">
       <c r="A72" s="12">
         <v>71</v>
       </c>
@@ -8092,25 +8383,29 @@
       <c r="E72" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" ht="15.75" customHeight="1">
+      <c r="F72" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> new Slot {SlotId(PK)(U,5)=71,DegreePlanId(FK)(U,5)=7256,Term(U,2)=5,CreditId(FK)(U,5)=664,Status(U,1)='P'},</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15.75" customHeight="1">
       <c r="B73" s="1"/>
     </row>
-    <row r="74" spans="1:5" ht="15.75" customHeight="1">
+    <row r="74" spans="1:6" ht="15.75" customHeight="1">
       <c r="B74" s="1"/>
     </row>
-    <row r="75" spans="1:5" ht="15.75" customHeight="1">
+    <row r="75" spans="1:6" ht="15.75" customHeight="1">
       <c r="B75" s="1"/>
     </row>
-    <row r="76" spans="1:5" ht="15.75" customHeight="1">
+    <row r="76" spans="1:6" ht="15.75" customHeight="1">
       <c r="B76" s="1"/>
     </row>
-    <row r="77" spans="1:5" ht="15.75" customHeight="1">
+    <row r="77" spans="1:6" ht="15.75" customHeight="1">
       <c r="B77" s="1"/>
     </row>
-    <row r="78" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="79" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="80" spans="1:5" ht="15.75" customHeight="1"/>
+    <row r="78" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="79" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="80" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -9040,8 +9335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9055,19 +9350,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -9305,7 +9600,7 @@
         <v>51</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:5">

</xml_diff>